<commit_message>
Code clean up and added quadratic basis function functionality.
</commit_message>
<xml_diff>
--- a/Finite Element Methods/SS Convection-Diffusion (generalised)/SSCD_Data_Combined.xlsx
+++ b/Finite Element Methods/SS Convection-Diffusion (generalised)/SSCD_Data_Combined.xlsx
@@ -1,29 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshi267\Data\Codes\NMCE_codes\Finite Element Methods\SS Convection-Diffusion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshi267\Data\Codes\NMCE_codes\Finite Element Methods\SS Convection-Diffusion (generalised)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1FBDDF5E-B3E3-4F9F-8F1D-CF4FDC12C625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147C4624-5324-4CE4-9129-2E8F86E7F66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="4" r:id="rId1"/>
     <sheet name="SSCD-Pe_0" sheetId="1" r:id="rId2"/>
     <sheet name="SSCD-Pe_5" sheetId="2" r:id="rId3"/>
     <sheet name="SSCD-Pe_50" sheetId="3" r:id="rId4"/>
+    <sheet name="SSCDVar-Pe_50" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>x</t>
   </si>
@@ -36,11 +50,20 @@
   <si>
     <t>c(x) Analytical</t>
   </si>
+  <si>
+    <t>C(x) Pe = 50</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>c(x) FEMVar</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -518,18 +541,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -628,14 +652,26 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -755,7 +791,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -803,7 +851,7 @@
             <c:numRef>
               <c:f>Compiled!$C$3:$C$13</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>-1.8027859110531901E-17</c:v>
@@ -823,19 +871,19 @@
                 <c:pt idx="5">
                   <c:v>7.2149643705463007E-2</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="General">
+                <c:pt idx="6">
                   <c:v>0.124305007244573</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="General">
+                <c:pt idx="7">
                   <c:v>0.211230613143089</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="General">
+                <c:pt idx="8">
                   <c:v>0.35610662297395002</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="General">
+                <c:pt idx="9">
                   <c:v>0.59756663935871901</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="10">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -875,7 +923,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -969,8 +1029,146 @@
           </c:extLst>
         </c:ser>
         <c:ser>
+          <c:idx val="6"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Compiled!$B$15:$B$16</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>c(x) FEMVar</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Compiled!$A$17:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.73333333333333339</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.82500000000000007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.88000000000000012</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.91666666666666674</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.94285714285714295</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.96250000000000013</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.97777777777777786</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Compiled!$B$17:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-2.26943890644721E-17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3.2763266644831497E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2190983625352999E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-8.49682038747233E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.2673685210432898E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0149132816862E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.87034611927998E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.14272192040371601</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.319138606339683</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.59999395318717796</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-77A9-4A0C-9B21-96500426D70B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>Compiled!$E$1:$E$2</c:f>
@@ -1090,7 +1288,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="4"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
               <c:f>Compiled!$F$1:$F$2</c:f>
@@ -1163,7 +1361,7 @@
             <c:numRef>
               <c:f>Compiled!$F$3:$F$13</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1223,7 +1421,7 @@
             <c15:filteredScatterSeries>
               <c15:ser>
                 <c:idx val="5"/>
-                <c:order val="5"/>
+                <c:order val="6"/>
                 <c:tx>
                   <c:strRef>
                     <c:extLst>
@@ -1606,7 +1804,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="l"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1636,6 +1834,372 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'SSCDVar-Pe_50'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C(x) Pe = 50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'SSCDVar-Pe_50'!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.73333333333333339</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.82500000000000007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.88000000000000012</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.91666666666666674</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.94285714285714295</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.96250000000000013</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.97777777777777786</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'SSCDVar-Pe_50'!$C$2:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-2.26943890644721E-17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3.2763266644831497E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2190983625352999E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-8.49682038747233E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.2673685210432898E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0149132816862E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.87034611927998E-2</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>0.14272192040371601</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>0.319138606339683</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>0.59999395318717796</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BD50-4FB8-9407-30B104244574}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2078195327"/>
+        <c:axId val="2082311791"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2078195327"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2082311791"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2082311791"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2078195327"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1720,6 +2284,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2236,20 +2840,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>34290</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>34290</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2257,6 +3377,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C43249B-EE76-D73A-5AAB-F4157DF0142F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5A06FCB-6A10-1998-E334-648283A0FDDF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2573,32 +3734,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2">
@@ -2620,14 +3784,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="B3" s="1">
         <v>2.2204460492503101E-16</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="5">
         <v>-1.8027859110531901E-17</v>
       </c>
       <c r="D3" s="1">
@@ -2636,23 +3800,23 @@
       <c r="E3" s="1">
         <v>0</v>
       </c>
-      <c r="F3" s="1">
-        <f>(EXP($F$2*A3)-1)/(EXP($F$2)-1)</f>
+      <c r="F3" s="5">
+        <f t="shared" ref="F3:F13" si="0">(EXP($F$2*A3)-1)/(EXP($F$2)-1)</f>
         <v>0</v>
       </c>
       <c r="G3" s="1">
-        <f>(EXP($G$2*A3)-1)/(EXP($G$2)-1)</f>
+        <f t="shared" ref="G3:G13" si="1">(EXP($G$2*A3)-1)/(EXP($G$2)-1)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.1</v>
       </c>
       <c r="B4">
         <v>0.1</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="5">
         <v>4.0556010688011599E-3</v>
       </c>
       <c r="D4" s="1">
@@ -2661,23 +3825,23 @@
       <c r="E4" s="1">
         <v>0.1</v>
       </c>
-      <c r="F4" s="1">
-        <f>(EXP($F$2*A4)-1)/(EXP($F$2)-1)</f>
+      <c r="F4" s="5">
+        <f t="shared" si="0"/>
         <v>4.4007012308088398E-3</v>
       </c>
       <c r="G4" s="1">
-        <f>(EXP($G$2*A4)-1)/(EXP($G$2)-1)</f>
+        <f t="shared" si="1"/>
         <v>2.8432310820697546E-20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.2</v>
       </c>
       <c r="B5">
         <v>0.2</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="5">
         <v>1.0814936183469801E-2</v>
       </c>
       <c r="D5" s="1">
@@ -2686,23 +3850,23 @@
       <c r="E5" s="1">
         <v>0.2</v>
       </c>
-      <c r="F5" s="1">
-        <f>(EXP($F$2*A5)-1)/(EXP($F$2)-1)</f>
+      <c r="F5" s="5">
+        <f t="shared" si="0"/>
         <v>1.1656230956039607E-2</v>
       </c>
       <c r="G5" s="1">
-        <f>(EXP($G$2*A5)-1)/(EXP($G$2)-1)</f>
+        <f t="shared" si="1"/>
         <v>4.2481613803067933E-18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.3</v>
       </c>
       <c r="B6">
         <v>0.3</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="5">
         <v>2.2080494707917502E-2</v>
       </c>
       <c r="D6" s="1">
@@ -2711,23 +3875,23 @@
       <c r="E6" s="1">
         <v>0.3</v>
       </c>
-      <c r="F6" s="1">
-        <f>(EXP($F$2*A6)-1)/(EXP($F$2)-1)</f>
+      <c r="F6" s="5">
+        <f t="shared" si="0"/>
         <v>2.361857714422463E-2</v>
       </c>
       <c r="G6" s="1">
-        <f>(EXP($G$2*A6)-1)/(EXP($G$2)-1)</f>
+        <f t="shared" si="1"/>
         <v>6.3051148313971422E-16</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.4</v>
       </c>
       <c r="B7">
         <v>0.4</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="5">
         <v>4.0856425581997098E-2</v>
       </c>
       <c r="D7" s="1">
@@ -2736,23 +3900,23 @@
       <c r="E7" s="1">
         <v>0.4</v>
       </c>
-      <c r="F7" s="1">
-        <f>(EXP($F$2*A7)-1)/(EXP($F$2)-1)</f>
+      <c r="F7" s="5">
+        <f t="shared" si="0"/>
         <v>4.3341151752163881E-2</v>
       </c>
       <c r="G7" s="1">
-        <f>(EXP($G$2*A7)-1)/(EXP($G$2)-1)</f>
+        <f t="shared" si="1"/>
         <v>9.3576229495526771E-14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.5</v>
       </c>
       <c r="B8">
         <v>0.5</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="5">
         <v>7.2149643705463007E-2</v>
       </c>
       <c r="D8" s="1">
@@ -2761,23 +3925,23 @@
       <c r="E8" s="1">
         <v>0.5</v>
       </c>
-      <c r="F8" s="1">
-        <f>(EXP($F$2*A8)-1)/(EXP($F$2)-1)</f>
+      <c r="F8" s="5">
+        <f t="shared" si="0"/>
         <v>7.5858180021243546E-2</v>
       </c>
       <c r="G8" s="1">
-        <f>(EXP($G$2*A8)-1)/(EXP($G$2)-1)</f>
+        <f t="shared" si="1"/>
         <v>1.3887943864771149E-11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.6</v>
       </c>
       <c r="B9">
         <v>0.6</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="5">
         <v>0.124305007244573</v>
       </c>
       <c r="D9" s="1">
@@ -2786,23 +3950,23 @@
       <c r="E9" s="1">
         <v>0.6</v>
       </c>
-      <c r="F9" s="1">
-        <f>(EXP($F$2*A9)-1)/(EXP($F$2)-1)</f>
+      <c r="F9" s="5">
+        <f t="shared" si="0"/>
         <v>0.1294696961884326</v>
       </c>
       <c r="G9" s="1">
-        <f>(EXP($G$2*A9)-1)/(EXP($G$2)-1)</f>
+        <f t="shared" si="1"/>
         <v>2.0611536224383651E-9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.7</v>
       </c>
       <c r="B10">
         <v>0.7</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="5">
         <v>0.211230613143089</v>
       </c>
       <c r="D10" s="1">
@@ -2811,23 +3975,23 @@
       <c r="E10" s="1">
         <v>0.7</v>
       </c>
-      <c r="F10" s="1">
-        <f>(EXP($F$2*A10)-1)/(EXP($F$2)-1)</f>
+      <c r="F10" s="5">
+        <f t="shared" si="0"/>
         <v>0.21786014324776093</v>
       </c>
       <c r="G10" s="1">
-        <f>(EXP($G$2*A10)-1)/(EXP($G$2)-1)</f>
+        <f t="shared" si="1"/>
         <v>3.0590232050182563E-7</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.8</v>
       </c>
       <c r="B11">
         <v>0.8</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="5">
         <v>0.35610662297395002</v>
       </c>
       <c r="D11">
@@ -2836,23 +4000,23 @@
       <c r="E11" s="1">
         <v>0.8</v>
       </c>
-      <c r="F11" s="1">
-        <f>(EXP($F$2*A11)-1)/(EXP($F$2)-1)</f>
+      <c r="F11" s="5">
+        <f t="shared" si="0"/>
         <v>0.36359135344116922</v>
       </c>
       <c r="G11" s="1">
-        <f>(EXP($G$2*A11)-1)/(EXP($G$2)-1)</f>
+        <f t="shared" si="1"/>
         <v>4.5399929762484861E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.9</v>
       </c>
       <c r="B12">
         <v>0.9</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="5">
         <v>0.59756663935871901</v>
       </c>
       <c r="D12">
@@ -2861,23 +4025,23 @@
       <c r="E12" s="1">
         <v>0.9</v>
       </c>
-      <c r="F12" s="1">
-        <f>(EXP($F$2*A12)-1)/(EXP($F$2)-1)</f>
+      <c r="F12" s="5">
+        <f t="shared" si="0"/>
         <v>0.6038614994919127</v>
       </c>
       <c r="G12" s="1">
-        <f>(EXP($G$2*A12)-1)/(EXP($G$2)-1)</f>
+        <f t="shared" si="1"/>
         <v>6.7379469990854679E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="5">
         <v>1</v>
       </c>
       <c r="D13">
@@ -2886,12 +4050,214 @@
       <c r="E13" s="1">
         <v>1</v>
       </c>
-      <c r="F13" s="1">
-        <f>(EXP($F$2*A13)-1)/(EXP($F$2)-1)</f>
+      <c r="F13" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G13" s="1">
-        <f>(EXP($G$2*A13)-1)/(EXP($G$2)-1)</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>-2.26943890644721E-17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B18">
+        <v>-3.2763266644831497E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.73333333333333339</v>
+      </c>
+      <c r="B19">
+        <v>1.2190983625352999E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0.82500000000000007</v>
+      </c>
+      <c r="B20">
+        <v>-8.49682038747233E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0.88000000000000012</v>
+      </c>
+      <c r="B21">
+        <v>4.2673685210432898E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0.91666666666666674</v>
+      </c>
+      <c r="B22">
+        <v>1.0149132816862E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.94285714285714295</v>
+      </c>
+      <c r="B23">
+        <v>4.87034611927998E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0.96250000000000013</v>
+      </c>
+      <c r="B24">
+        <v>0.14272192040371601</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0.97777777777777786</v>
+      </c>
+      <c r="B25">
+        <v>0.319138606339683</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0.9900000000000001</v>
+      </c>
+      <c r="B26">
+        <v>0.59999395318717796</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F32" s="5">
+        <f>(EXP($F$2*E32)-1)/(EXP($F$2)-1)</f>
+        <v>9.9330561622379854E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>0.73333333333333339</v>
+      </c>
+      <c r="F33" s="5">
+        <f t="shared" ref="F33:F41" si="2">(EXP($F$2*E33)-1)/(EXP($F$2)-1)</f>
+        <v>0.25860163522868918</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>0.82500000000000007</v>
+      </c>
+      <c r="F34" s="5">
+        <f t="shared" si="2"/>
+        <v>0.41290621285724816</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>0.88000000000000012</v>
+      </c>
+      <c r="F35" s="5">
+        <f t="shared" si="2"/>
+        <v>0.54575092993554841</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>0.91666666666666674</v>
+      </c>
+      <c r="F36" s="5">
+        <f t="shared" si="2"/>
+        <v>0.65692903622963417</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>0.94285714285714295</v>
+      </c>
+      <c r="F37" s="5">
+        <f t="shared" si="2"/>
+        <v>0.74979140079512818</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>0.96250000000000013</v>
+      </c>
+      <c r="F38" s="5">
+        <f t="shared" si="2"/>
+        <v>0.82786931071911041</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>0.97777777777777786</v>
+      </c>
+      <c r="F39" s="5">
+        <f t="shared" si="2"/>
+        <v>0.89412594302992765</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>0.9900000000000001</v>
+      </c>
+      <c r="F40" s="5">
+        <f t="shared" si="2"/>
+        <v>0.95089858174694508</v>
+      </c>
+    </row>
+    <row r="41" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41" s="5">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -2906,16 +4272,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B11"/>
+      <selection activeCell="B1" sqref="B1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -2924,7 +4290,7 @@
       </c>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -2932,7 +4298,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.2</v>
       </c>
@@ -2941,7 +4307,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.3</v>
       </c>
@@ -2950,7 +4316,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.4</v>
       </c>
@@ -2959,7 +4325,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.5</v>
       </c>
@@ -2968,7 +4334,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.6</v>
       </c>
@@ -2977,7 +4343,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.7</v>
       </c>
@@ -2986,7 +4352,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.8</v>
       </c>
@@ -2995,7 +4361,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.9</v>
       </c>
@@ -3004,7 +4370,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -3018,16 +4384,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -3035,7 +4401,7 @@
         <v>-1.8027859110531901E-17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -3043,7 +4409,7 @@
         <v>4.0556010688011599E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.2</v>
       </c>
@@ -3051,7 +4417,7 @@
         <v>1.0814936183469801E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.3</v>
       </c>
@@ -3059,7 +4425,7 @@
         <v>2.2080494707917502E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.4</v>
       </c>
@@ -3067,7 +4433,7 @@
         <v>4.0856425581997098E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.5</v>
       </c>
@@ -3075,7 +4441,7 @@
         <v>7.2149643705463007E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.6</v>
       </c>
@@ -3083,7 +4449,7 @@
         <v>0.124305007244573</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.7</v>
       </c>
@@ -3091,7 +4457,7 @@
         <v>0.211230613143089</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.8</v>
       </c>
@@ -3099,7 +4465,7 @@
         <v>0.35610662297395002</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.9</v>
       </c>
@@ -3107,7 +4473,7 @@
         <v>0.59756663935871901</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -3121,16 +4487,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -3138,7 +4504,7 @@
         <v>1.5286125444138799E-17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -3146,7 +4512,7 @@
         <v>-6.9695010413706995E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.2</v>
       </c>
@@ -3154,7 +4520,7 @@
         <v>9.2926680551612905E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.3</v>
       </c>
@@ -3162,7 +4528,7 @@
         <v>-2.865239317008E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.4</v>
       </c>
@@ -3170,7 +4536,7 @@
         <v>5.9886083022149704E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.5</v>
       </c>
@@ -3178,7 +4544,7 @@
         <v>-1.46703694759719E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.6</v>
       </c>
@@ -3186,7 +4552,7 @@
         <v>3.3533912006464203E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.7</v>
       </c>
@@ -3194,7 +4560,7 @@
         <v>-7.8942744785886906E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.8</v>
       </c>
@@ -3202,7 +4568,7 @@
         <v>0.18350278772959899</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.9</v>
       </c>
@@ -3210,7 +4576,7 @@
         <v>-0.42887012147320103</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -3221,4 +4587,163 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0223A4BA-9DEA-47E1-9589-2AD9988EE6DF}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>1.1-1.1/A2</f>
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>-2.26943890644721E-17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B12" si="0">1.1-1.1/A3</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-3.2763266644831497E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>0.73333333333333339</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1.2190983625352999E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>0.82500000000000007</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-8.49682038747233E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>0.88000000000000012</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4.2673685210432898E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>0.91666666666666674</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1.0149132816862E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>0.94285714285714295</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4.87034611927998E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>0.96250000000000013</v>
+      </c>
+      <c r="C9">
+        <v>0.14272192040371601</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>0.97777777777777786</v>
+      </c>
+      <c r="C10">
+        <v>0.319138606339683</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>0.9900000000000001</v>
+      </c>
+      <c r="C11">
+        <v>0.59999395318717796</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Misclaneous improvements to SSCD codes.
1. The SS Convection Diffusion as well as SSCDR codes are obsolete.
2. Refer to 1D (generalised) folder for most general 1D linear code.
3. These other codes are just there to track the generalization process by adding layers of complxity with each new probelem.
</commit_message>
<xml_diff>
--- a/Finite Element Methods/SS Convection-Diffusion (generalised)/SSCD_Data_Combined.xlsx
+++ b/Finite Element Methods/SS Convection-Diffusion (generalised)/SSCD_Data_Combined.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshi267\Data\Codes\NMCE_codes\Finite Element Methods\SS Convection-Diffusion (generalised)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147C4624-5324-4CE4-9129-2E8F86E7F66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B454D6C3-B571-4CCB-BEBE-2564BAA9C272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="4" r:id="rId1"/>
@@ -64,6 +64,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.0E+00"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -541,7 +544,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -550,10 +553,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1121,7 +1125,7 @@
             <c:numRef>
               <c:f>Compiled!$B$17:$B$27</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0E+00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>-2.26943890644721E-17</c:v>
@@ -1512,7 +1516,7 @@
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
-                      <c:formatCode>0.00E+00</c:formatCode>
+                      <c:formatCode>General</c:formatCode>
                       <c:ptCount val="11"/>
                       <c:pt idx="0">
                         <c:v>0</c:v>
@@ -3738,30 +3742,31 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -3780,18 +3785,18 @@
       <c r="F2">
         <v>5</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="4">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="B3" s="1">
         <v>2.2204460492503101E-16</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>-1.8027859110531901E-17</v>
       </c>
       <c r="D3" s="1">
@@ -3800,23 +3805,23 @@
       <c r="E3" s="1">
         <v>0</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <f t="shared" ref="F3:F13" si="0">(EXP($F$2*A3)-1)/(EXP($F$2)-1)</f>
         <v>0</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="4">
         <f t="shared" ref="G3:G13" si="1">(EXP($G$2*A3)-1)/(EXP($G$2)-1)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.1</v>
       </c>
       <c r="B4">
         <v>0.1</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>4.0556010688011599E-3</v>
       </c>
       <c r="D4" s="1">
@@ -3825,23 +3830,23 @@
       <c r="E4" s="1">
         <v>0.1</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <f t="shared" si="0"/>
         <v>4.4007012308088398E-3</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="4">
         <f t="shared" si="1"/>
         <v>2.8432310820697546E-20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.2</v>
       </c>
       <c r="B5">
         <v>0.2</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>1.0814936183469801E-2</v>
       </c>
       <c r="D5" s="1">
@@ -3850,23 +3855,23 @@
       <c r="E5" s="1">
         <v>0.2</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <f t="shared" si="0"/>
         <v>1.1656230956039607E-2</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="4">
         <f t="shared" si="1"/>
         <v>4.2481613803067933E-18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0.3</v>
       </c>
       <c r="B6">
         <v>0.3</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>2.2080494707917502E-2</v>
       </c>
       <c r="D6" s="1">
@@ -3875,23 +3880,23 @@
       <c r="E6" s="1">
         <v>0.3</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <f t="shared" si="0"/>
         <v>2.361857714422463E-2</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="4">
         <f t="shared" si="1"/>
         <v>6.3051148313971422E-16</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0.4</v>
       </c>
       <c r="B7">
         <v>0.4</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>4.0856425581997098E-2</v>
       </c>
       <c r="D7" s="1">
@@ -3900,23 +3905,23 @@
       <c r="E7" s="1">
         <v>0.4</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <f t="shared" si="0"/>
         <v>4.3341151752163881E-2</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="4">
         <f t="shared" si="1"/>
         <v>9.3576229495526771E-14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0.5</v>
       </c>
       <c r="B8">
         <v>0.5</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>7.2149643705463007E-2</v>
       </c>
       <c r="D8" s="1">
@@ -3925,23 +3930,23 @@
       <c r="E8" s="1">
         <v>0.5</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <f t="shared" si="0"/>
         <v>7.5858180021243546E-2</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="4">
         <f t="shared" si="1"/>
         <v>1.3887943864771149E-11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0.6</v>
       </c>
       <c r="B9">
         <v>0.6</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>0.124305007244573</v>
       </c>
       <c r="D9" s="1">
@@ -3950,23 +3955,23 @@
       <c r="E9" s="1">
         <v>0.6</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <f t="shared" si="0"/>
         <v>0.1294696961884326</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="4">
         <f t="shared" si="1"/>
         <v>2.0611536224383651E-9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0.7</v>
       </c>
       <c r="B10">
         <v>0.7</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>0.211230613143089</v>
       </c>
       <c r="D10" s="1">
@@ -3975,23 +3980,23 @@
       <c r="E10" s="1">
         <v>0.7</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <f t="shared" si="0"/>
         <v>0.21786014324776093</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="4">
         <f t="shared" si="1"/>
         <v>3.0590232050182563E-7</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0.8</v>
       </c>
       <c r="B11">
         <v>0.8</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>0.35610662297395002</v>
       </c>
       <c r="D11">
@@ -4000,23 +4005,23 @@
       <c r="E11" s="1">
         <v>0.8</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <f t="shared" si="0"/>
         <v>0.36359135344116922</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="4">
         <f t="shared" si="1"/>
         <v>4.5399929762484861E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0.9</v>
       </c>
       <c r="B12">
         <v>0.9</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>0.59756663935871901</v>
       </c>
       <c r="D12">
@@ -4025,23 +4030,23 @@
       <c r="E12" s="1">
         <v>0.9</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <f t="shared" si="0"/>
         <v>0.6038614994919127</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="4">
         <f t="shared" si="1"/>
         <v>6.7379469990854679E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>1</v>
       </c>
       <c r="D13">
@@ -4050,16 +4055,16 @@
       <c r="E13" s="1">
         <v>1</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="4">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -4067,7 +4072,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -4075,188 +4080,188 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>0</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="6">
         <v>-2.26943890644721E-17</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0.55000000000000004</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="6">
         <v>-3.2763266644831497E-5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0.73333333333333339</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="6">
         <v>1.2190983625352999E-5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0.82500000000000007</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="6">
         <v>-8.49682038747233E-5</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0.88000000000000012</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="6">
         <v>4.2673685210432898E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>0.91666666666666674</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="6">
         <v>1.0149132816862E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>0.94285714285714295</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="6">
         <v>4.87034611927998E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>0.96250000000000013</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="6">
         <v>0.14272192040371601</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>0.97777777777777786</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="6">
         <v>0.319138606339683</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>0.9900000000000001</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="6">
         <v>0.59999395318717796</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E31">
         <v>0</v>
       </c>
-      <c r="F31" s="5">
+      <c r="F31" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E32">
         <v>0.55000000000000004</v>
       </c>
-      <c r="F32" s="5">
+      <c r="F32" s="4">
         <f>(EXP($F$2*E32)-1)/(EXP($F$2)-1)</f>
         <v>9.9330561622379854E-2</v>
       </c>
     </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E33">
         <v>0.73333333333333339</v>
       </c>
-      <c r="F33" s="5">
+      <c r="F33" s="4">
         <f t="shared" ref="F33:F41" si="2">(EXP($F$2*E33)-1)/(EXP($F$2)-1)</f>
         <v>0.25860163522868918</v>
       </c>
     </row>
-    <row r="34" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E34">
         <v>0.82500000000000007</v>
       </c>
-      <c r="F34" s="5">
+      <c r="F34" s="4">
         <f t="shared" si="2"/>
         <v>0.41290621285724816</v>
       </c>
     </row>
-    <row r="35" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E35">
         <v>0.88000000000000012</v>
       </c>
-      <c r="F35" s="5">
+      <c r="F35" s="4">
         <f t="shared" si="2"/>
         <v>0.54575092993554841</v>
       </c>
     </row>
-    <row r="36" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E36">
         <v>0.91666666666666674</v>
       </c>
-      <c r="F36" s="5">
+      <c r="F36" s="4">
         <f t="shared" si="2"/>
         <v>0.65692903622963417</v>
       </c>
     </row>
-    <row r="37" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E37">
         <v>0.94285714285714295</v>
       </c>
-      <c r="F37" s="5">
+      <c r="F37" s="4">
         <f t="shared" si="2"/>
         <v>0.74979140079512818</v>
       </c>
     </row>
-    <row r="38" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E38">
         <v>0.96250000000000013</v>
       </c>
-      <c r="F38" s="5">
+      <c r="F38" s="4">
         <f t="shared" si="2"/>
         <v>0.82786931071911041</v>
       </c>
     </row>
-    <row r="39" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E39">
         <v>0.97777777777777786</v>
       </c>
-      <c r="F39" s="5">
+      <c r="F39" s="4">
         <f t="shared" si="2"/>
         <v>0.89412594302992765</v>
       </c>
     </row>
-    <row r="40" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E40">
         <v>0.9900000000000001</v>
       </c>
-      <c r="F40" s="5">
+      <c r="F40" s="4">
         <f t="shared" si="2"/>
         <v>0.95089858174694508</v>
       </c>
     </row>
-    <row r="41" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E41">
         <v>1</v>
       </c>
-      <c r="F41" s="5">
+      <c r="F41" s="4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -4279,9 +4284,9 @@
       <selection activeCell="B1" sqref="B1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>0</v>
       </c>
@@ -4290,7 +4295,7 @@
       </c>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -4298,7 +4303,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0.2</v>
       </c>
@@ -4307,7 +4312,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.3</v>
       </c>
@@ -4316,7 +4321,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.4</v>
       </c>
@@ -4325,7 +4330,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0.5</v>
       </c>
@@ -4334,7 +4339,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0.6</v>
       </c>
@@ -4343,7 +4348,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0.7</v>
       </c>
@@ -4352,7 +4357,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0.8</v>
       </c>
@@ -4361,7 +4366,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0.9</v>
       </c>
@@ -4370,7 +4375,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -4391,9 +4396,9 @@
       <selection activeCell="B1" sqref="B1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>0</v>
       </c>
@@ -4401,7 +4406,7 @@
         <v>-1.8027859110531901E-17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -4409,7 +4414,7 @@
         <v>4.0556010688011599E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0.2</v>
       </c>
@@ -4417,7 +4422,7 @@
         <v>1.0814936183469801E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.3</v>
       </c>
@@ -4425,7 +4430,7 @@
         <v>2.2080494707917502E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.4</v>
       </c>
@@ -4433,7 +4438,7 @@
         <v>4.0856425581997098E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0.5</v>
       </c>
@@ -4441,7 +4446,7 @@
         <v>7.2149643705463007E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0.6</v>
       </c>
@@ -4449,7 +4454,7 @@
         <v>0.124305007244573</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0.7</v>
       </c>
@@ -4457,7 +4462,7 @@
         <v>0.211230613143089</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0.8</v>
       </c>
@@ -4465,7 +4470,7 @@
         <v>0.35610662297395002</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0.9</v>
       </c>
@@ -4473,7 +4478,7 @@
         <v>0.59756663935871901</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -4494,9 +4499,9 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>0</v>
       </c>
@@ -4504,7 +4509,7 @@
         <v>1.5286125444138799E-17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -4512,7 +4517,7 @@
         <v>-6.9695010413706995E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0.2</v>
       </c>
@@ -4520,7 +4525,7 @@
         <v>9.2926680551612905E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.3</v>
       </c>
@@ -4528,7 +4533,7 @@
         <v>-2.865239317008E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.4</v>
       </c>
@@ -4536,7 +4541,7 @@
         <v>5.9886083022149704E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0.5</v>
       </c>
@@ -4544,7 +4549,7 @@
         <v>-1.46703694759719E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0.6</v>
       </c>
@@ -4552,7 +4557,7 @@
         <v>3.3533912006464203E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0.7</v>
       </c>
@@ -4560,7 +4565,7 @@
         <v>-7.8942744785886906E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0.8</v>
       </c>
@@ -4568,7 +4573,7 @@
         <v>0.18350278772959899</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0.9</v>
       </c>
@@ -4576,7 +4581,7 @@
         <v>-0.42887012147320103</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -4597,9 +4602,9 @@
       <selection activeCell="B1" sqref="B1:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -4610,7 +4615,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4622,7 +4627,7 @@
         <v>-2.26943890644721E-17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4634,7 +4639,7 @@
         <v>-3.2763266644831497E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4646,7 +4651,7 @@
         <v>1.2190983625352999E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4658,7 +4663,7 @@
         <v>-8.49682038747233E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4670,7 +4675,7 @@
         <v>4.2673685210432898E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4682,7 +4687,7 @@
         <v>1.0149132816862E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4694,7 +4699,7 @@
         <v>4.87034611927998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4706,7 +4711,7 @@
         <v>0.14272192040371601</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4718,7 +4723,7 @@
         <v>0.319138606339683</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4730,7 +4735,7 @@
         <v>0.59999395318717796</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>

</xml_diff>